<commit_message>
visualizing loss landscapes in backprop vs btsp
</commit_message>
<xml_diff>
--- a/notebooks/logbook.xlsx
+++ b/notebooks/logbook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ag1880/Github_repos/Milstein-Lab/dentate_circuit_model/notebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ag1880/Github_repos/Milstein-Lab/dentate_circuit_learning/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D464AD-C8C5-FA47-A516-6A9BD865A5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917F7E43-E15A-C247-AEA5-064465D6ADA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{433C4AE9-2C5A-E840-91F3-D0595A9D2CC0}"/>
   </bookViews>
@@ -864,10 +864,10 @@
   <dimension ref="A1:P78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A70" sqref="A70"/>
+      <selection pane="bottomRight" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>